<commit_message>
RSI fast slow 10/31
</commit_message>
<xml_diff>
--- a/pdfcreater/excel/RSI横截面_纯多头_hsi_OUTPUT.xlsx
+++ b/pdfcreater/excel/RSI横截面_纯多头_hsi_OUTPUT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meiconte\Desktop\pdfcreater\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meiconte\Documents\RH\pdfcreater\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>